<commit_message>
Forbedret valg ved flere kand med like mnage stemmer.
</commit_message>
<xml_diff>
--- a/Work in progress/Stemmesedler.xlsx
+++ b/Work in progress/Stemmesedler.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eirik\OneDrive\VT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eirik\OneDrive\GitRepo\Preferansevalg_VelferdstingetVest\Work in progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="6731662E5A86D4C75C6F0E11B3158EE63E5E3BFC" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{58881418-6584-48B0-8B25-081B0A9FE506}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="6731662E5A86D4C75C6F0E11B3158EE63E5E3BFC" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{F93F07FA-BDF5-42A7-ADA2-E2186FB3C8DF}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{F4DDF6A2-C2DA-49A5-A223-48FB2C433CB8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Kandidat / Stemme</t>
   </si>
@@ -109,21 +109,6 @@
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>I</t>
   </si>
   <si>
     <t>B</t>
@@ -515,13 +500,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45921AFB-57CF-4B80-A9BF-42009DE883CC}">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,13 +598,13 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -628,90 +613,78 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R2">
         <v>1</v>
       </c>
       <c r="S2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>1</v>
-      </c>
-      <c r="V2">
-        <v>3</v>
-      </c>
-      <c r="W2">
-        <v>3</v>
-      </c>
-      <c r="X2">
-        <v>4</v>
-      </c>
-      <c r="Y2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -720,46 +693,34 @@
         <v>2</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>4</v>
-      </c>
-      <c r="V3">
-        <v>2</v>
-      </c>
-      <c r="W3">
-        <v>2</v>
-      </c>
-      <c r="X3">
-        <v>1</v>
-      </c>
-      <c r="Y3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -767,76 +728,64 @@
         <v>26</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="O4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="R4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="S4">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="U4">
-        <v>7</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>8</v>
-      </c>
-      <c r="Y4">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -853,7 +802,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -868,13 +817,13 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -883,422 +832,25 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R5">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S5">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="T5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="U5">
-        <v>5</v>
-      </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="W5">
-        <v>1</v>
-      </c>
-      <c r="X5">
-        <v>7</v>
-      </c>
-      <c r="Y5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6">
-        <v>5</v>
-      </c>
-      <c r="K6">
-        <v>4</v>
-      </c>
-      <c r="L6">
-        <v>3</v>
-      </c>
-      <c r="M6">
-        <v>4</v>
-      </c>
-      <c r="N6">
-        <v>4</v>
-      </c>
-      <c r="O6">
-        <v>2</v>
-      </c>
-      <c r="P6">
-        <v>3</v>
-      </c>
-      <c r="Q6">
-        <v>3</v>
-      </c>
-      <c r="R6">
-        <v>3</v>
-      </c>
-      <c r="S6">
-        <v>2</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6">
-        <v>3</v>
-      </c>
-      <c r="V6">
-        <v>0</v>
-      </c>
-      <c r="W6">
-        <v>0</v>
-      </c>
-      <c r="X6">
-        <v>2</v>
-      </c>
-      <c r="Y6">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-      <c r="E7">
-        <v>6</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
-        <v>5</v>
-      </c>
-      <c r="O7">
-        <v>5</v>
-      </c>
-      <c r="P7">
-        <v>4</v>
-      </c>
-      <c r="Q7">
-        <v>6</v>
-      </c>
-      <c r="R7">
-        <v>6</v>
-      </c>
-      <c r="S7">
-        <v>5</v>
-      </c>
-      <c r="T7">
-        <v>9</v>
-      </c>
-      <c r="U7">
-        <v>0</v>
-      </c>
-      <c r="V7">
-        <v>0</v>
-      </c>
-      <c r="W7">
-        <v>0</v>
-      </c>
-      <c r="X7">
-        <v>6</v>
-      </c>
-      <c r="Y7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8">
-        <v>8</v>
-      </c>
-      <c r="P8">
-        <v>5</v>
-      </c>
-      <c r="Q8">
-        <v>8</v>
-      </c>
-      <c r="R8">
-        <v>7</v>
-      </c>
-      <c r="S8">
-        <v>9</v>
-      </c>
-      <c r="T8">
-        <v>7</v>
-      </c>
-      <c r="U8">
-        <v>6</v>
-      </c>
-      <c r="V8">
-        <v>5</v>
-      </c>
-      <c r="W8">
-        <v>5</v>
-      </c>
-      <c r="X8">
-        <v>5</v>
-      </c>
-      <c r="Y8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>4</v>
-      </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9">
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>4</v>
-      </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
-      <c r="L9">
-        <v>4</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9">
-        <v>1</v>
-      </c>
-      <c r="O9">
-        <v>3</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>5</v>
-      </c>
-      <c r="R9">
-        <v>2</v>
-      </c>
-      <c r="S9">
-        <v>1</v>
-      </c>
-      <c r="T9">
-        <v>2</v>
-      </c>
-      <c r="U9">
-        <v>2</v>
-      </c>
-      <c r="V9">
-        <v>4</v>
-      </c>
-      <c r="W9">
-        <v>4</v>
-      </c>
-      <c r="X9">
-        <v>3</v>
-      </c>
-      <c r="Y9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>5</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10">
-        <v>4</v>
-      </c>
-      <c r="I10">
-        <v>3</v>
-      </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>6</v>
-      </c>
-      <c r="P10">
-        <v>2</v>
-      </c>
-      <c r="Q10">
-        <v>7</v>
-      </c>
-      <c r="R10">
-        <v>9</v>
-      </c>
-      <c r="S10">
-        <v>8</v>
-      </c>
-      <c r="T10">
-        <v>5</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
-      <c r="X10">
-        <v>9</v>
-      </c>
-      <c r="Y10">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resultat kommer i egen mappe med tidsstempel. Jobber med å forbedre Resultat til en txt-fil.
</commit_message>
<xml_diff>
--- a/Work in progress/Stemmesedler.xlsx
+++ b/Work in progress/Stemmesedler.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eirik\OneDrive\GitRepo\Preferansevalg_VelferdstingetVest\Work in progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eirik\OneDrive\VT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="6731662E5A86D4C75C6F0E11B3158EE63E5E3BFC" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{F93F07FA-BDF5-42A7-ADA2-E2186FB3C8DF}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="6731662E5A86D4C75C6F0E11B3158EE63E5E3BFC" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{58881418-6584-48B0-8B25-081B0A9FE506}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7530" xr2:uid="{F4DDF6A2-C2DA-49A5-A223-48FB2C433CB8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Kandidat / Stemme</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
   <si>
     <t>B</t>
@@ -500,13 +515,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45921AFB-57CF-4B80-A9BF-42009DE883CC}">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H19" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,13 +613,13 @@
         <v>25</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -613,78 +628,90 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="P2">
         <v>1</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R2">
         <v>1</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="T2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="V2">
+        <v>3</v>
+      </c>
+      <c r="W2">
+        <v>3</v>
+      </c>
+      <c r="X2">
+        <v>4</v>
+      </c>
+      <c r="Y2">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F3">
         <v>2</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -693,34 +720,46 @@
         <v>2</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="S3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="T3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="V3">
+        <v>2</v>
+      </c>
+      <c r="W3">
+        <v>2</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -728,64 +767,76 @@
         <v>26</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="R4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="S4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>8</v>
+      </c>
+      <c r="Y4">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -802,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -817,13 +868,13 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -832,25 +883,422 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="T5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="U5">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>7</v>
+      </c>
+      <c r="Y5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>3</v>
+      </c>
+      <c r="Q6">
+        <v>3</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="S6">
+        <v>2</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>3</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>2</v>
+      </c>
+      <c r="Y6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <v>6</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <v>9</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>6</v>
+      </c>
+      <c r="Y7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>8</v>
+      </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <v>8</v>
+      </c>
+      <c r="R8">
+        <v>7</v>
+      </c>
+      <c r="S8">
+        <v>9</v>
+      </c>
+      <c r="T8">
+        <v>7</v>
+      </c>
+      <c r="U8">
+        <v>6</v>
+      </c>
+      <c r="V8">
+        <v>5</v>
+      </c>
+      <c r="W8">
+        <v>5</v>
+      </c>
+      <c r="X8">
+        <v>5</v>
+      </c>
+      <c r="Y8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>3</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>5</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <v>2</v>
+      </c>
+      <c r="U9">
+        <v>2</v>
+      </c>
+      <c r="V9">
+        <v>4</v>
+      </c>
+      <c r="W9">
+        <v>4</v>
+      </c>
+      <c r="X9">
+        <v>3</v>
+      </c>
+      <c r="Y9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>6</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10">
+        <v>7</v>
+      </c>
+      <c r="R10">
+        <v>9</v>
+      </c>
+      <c r="S10">
+        <v>8</v>
+      </c>
+      <c r="T10">
+        <v>5</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>9</v>
+      </c>
+      <c r="Y10">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>